<commit_message>
Deployed 1990a985 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/parameters.xlsx
+++ b/Manual/source/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="25"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="307">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -443,7 +443,7 @@
     <t xml:space="preserve">2 x 6pin WEIDMÜLLER  SLS 5.08/06/180FI </t>
   </si>
   <si>
-    <t xml:space="preserve">400 VAC/50Hz 6A</t>
+    <t xml:space="preserve">3 x 400 VAC/50Hz 6A</t>
   </si>
   <si>
     <t xml:space="preserve">1,68 kVA</t>
@@ -512,7 +512,7 @@
     <t xml:space="preserve">24 VDC ± 10 %, 2 A*</t>
   </si>
   <si>
-    <t xml:space="preserve">140-600 VDC</t>
+    <t xml:space="preserve">0 ~ 560 VDC</t>
   </si>
   <si>
     <t xml:space="preserve">3,4 kVA</t>
@@ -564,9 +564,6 @@
   </si>
   <si>
     <t xml:space="preserve">150 W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24-560 VDC</t>
   </si>
   <si>
     <t xml:space="preserve">33,6 kVA</t>
@@ -2643,8 +2640,8 @@
   </sheetPr>
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2872,7 +2869,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3134,7 +3131,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4156,7 +4153,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4397,7 +4394,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4638,7 +4635,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4879,7 +4876,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4909,7 +4906,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4917,7 +4914,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4933,7 +4930,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4949,7 +4946,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5053,7 +5050,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5061,7 +5058,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5077,7 +5074,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5106,7 +5103,7 @@
         <v>122</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -5148,16 +5145,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>168</v>
@@ -5166,28 +5163,28 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>185</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>187</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -5202,37 +5199,37 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>193</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -5256,7 +5253,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -5264,18 +5261,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5291,12 +5288,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -5304,7 +5301,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>128</v>
@@ -5312,18 +5309,18 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -5365,43 +5362,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>49</v>
@@ -5413,31 +5410,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>166</v>
@@ -5446,10 +5443,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -5473,7 +5470,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -5481,18 +5478,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5508,12 +5505,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -5529,34 +5526,34 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -5577,8 +5574,8 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L38" activeCellId="0" sqref="L38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5606,16 +5603,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>49</v>
@@ -5624,16 +5621,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>49</v>
@@ -5642,7 +5639,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>59</v>
@@ -5654,22 +5651,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -5678,7 +5675,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>170</v>
@@ -5687,10 +5684,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C12" s="4"/>
     </row>
@@ -5714,7 +5711,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -5722,18 +5719,18 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5749,12 +5746,12 @@
         <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>1</v>
@@ -5765,47 +5762,47 @@
         <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -5847,28 +5844,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -5895,19 +5892,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="C9" s="4"/>
     </row>
@@ -5922,28 +5919,28 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="C13" s="4"/>
     </row>
@@ -5961,16 +5958,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="C16" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>1</v>
@@ -5978,10 +5975,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5989,15 +5986,15 @@
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -6039,28 +6036,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -6114,10 +6111,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -6135,10 +6132,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C14" s="4"/>
     </row>
@@ -6147,7 +6144,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -6156,7 +6153,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>39</v>
@@ -6167,7 +6164,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6233,28 +6230,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -6308,10 +6305,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -6329,10 +6326,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C14" s="4"/>
     </row>
@@ -6341,7 +6338,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -6353,7 +6350,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6629,107 +6626,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6737,16 +6734,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>2.05</v>
@@ -6772,16 +6769,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2.05</v>
@@ -6807,16 +6804,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>2.05</v>
@@ -6842,16 +6839,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>2.05</v>
@@ -6877,16 +6874,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>2.05</v>
@@ -6912,16 +6909,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2.05</v>
@@ -6947,16 +6944,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1.25</v>
@@ -6982,16 +6979,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>1.25</v>
@@ -7048,89 +7045,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="H3" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7150,7 +7147,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>300</v>
@@ -7179,7 +7176,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>300</v>
@@ -7208,7 +7205,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>300</v>
@@ -7237,7 +7234,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>300</v>
@@ -7266,7 +7263,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>300</v>
@@ -7295,7 +7292,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>300</v>
@@ -7339,44 +7336,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>275</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7384,7 +7381,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>11</v>
@@ -7398,7 +7395,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>11</v>

</xml_diff>

<commit_message>
Deployed 22e3023e with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/parameters.xlsx
+++ b/Manual/source/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,25 +21,26 @@
     <sheet name="TGZ-S-48-100_425" sheetId="11" state="visible" r:id="rId13"/>
     <sheet name="TGZ-S-48-100_425-O" sheetId="12" state="visible" r:id="rId14"/>
     <sheet name="TGZ-S-230-5_15" sheetId="13" state="visible" r:id="rId15"/>
-    <sheet name="TGZ-D-320-5_10" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="TGZ-D-320-5_15" sheetId="15" state="visible" r:id="rId17"/>
-    <sheet name="TGZ-S-400-3_9" sheetId="16" state="visible" r:id="rId18"/>
-    <sheet name="TGZ-S-400-7_15" sheetId="17" state="visible" r:id="rId19"/>
-    <sheet name="TGZ-S-400-10_20" sheetId="18" state="visible" r:id="rId20"/>
-    <sheet name="TGZ-S-400-14_30" sheetId="19" state="visible" r:id="rId21"/>
-    <sheet name="TGZ-D-560-3_9" sheetId="20" state="visible" r:id="rId22"/>
-    <sheet name="TGZ-D-560-7_15" sheetId="21" state="visible" r:id="rId23"/>
-    <sheet name="TGZ-D-560-10_20" sheetId="22" state="visible" r:id="rId24"/>
-    <sheet name="TGZ-D-560-30_50" sheetId="23" state="visible" r:id="rId25"/>
-    <sheet name="TGS-320-10_15" sheetId="24" state="visible" r:id="rId26"/>
-    <sheet name="TGS-560-25_50" sheetId="25" state="visible" r:id="rId27"/>
-    <sheet name="TGS-560-50_100" sheetId="26" state="visible" r:id="rId28"/>
-    <sheet name="TGMmini" sheetId="27" state="visible" r:id="rId29"/>
-    <sheet name="TGMcontroller" sheetId="28" state="visible" r:id="rId30"/>
-    <sheet name="TGZpMotion" sheetId="29" state="visible" r:id="rId31"/>
-    <sheet name="commonHW_DI" sheetId="30" state="visible" r:id="rId32"/>
-    <sheet name="commonHW_DO" sheetId="31" state="visible" r:id="rId33"/>
-    <sheet name="commonHW_AI" sheetId="32" state="visible" r:id="rId34"/>
+    <sheet name="TGZ-S-230-5_15-UNI-RI" sheetId="14" state="visible" r:id="rId16"/>
+    <sheet name="TGZ-D-320-5_10" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="TGZ-D-320-5_15" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="TGZ-S-400-3_9" sheetId="17" state="visible" r:id="rId19"/>
+    <sheet name="TGZ-S-400-7_15" sheetId="18" state="visible" r:id="rId20"/>
+    <sheet name="TGZ-S-400-10_20" sheetId="19" state="visible" r:id="rId21"/>
+    <sheet name="TGZ-S-400-14_30" sheetId="20" state="visible" r:id="rId22"/>
+    <sheet name="TGZ-D-560-3_9" sheetId="21" state="visible" r:id="rId23"/>
+    <sheet name="TGZ-D-560-7_15" sheetId="22" state="visible" r:id="rId24"/>
+    <sheet name="TGZ-D-560-10_20" sheetId="23" state="visible" r:id="rId25"/>
+    <sheet name="TGZ-D-560-30_50" sheetId="24" state="visible" r:id="rId26"/>
+    <sheet name="TGS-320-10_15" sheetId="25" state="visible" r:id="rId27"/>
+    <sheet name="TGS-560-25_50" sheetId="26" state="visible" r:id="rId28"/>
+    <sheet name="TGS-560-50_100" sheetId="27" state="visible" r:id="rId29"/>
+    <sheet name="TGMmini" sheetId="28" state="visible" r:id="rId30"/>
+    <sheet name="TGMcontroller" sheetId="29" state="visible" r:id="rId31"/>
+    <sheet name="TGZpMotion" sheetId="30" state="visible" r:id="rId32"/>
+    <sheet name="commonHW_DI" sheetId="31" state="visible" r:id="rId33"/>
+    <sheet name="commonHW_DO" sheetId="32" state="visible" r:id="rId34"/>
+    <sheet name="commonHW_AI" sheetId="33" state="visible" r:id="rId35"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="313">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -423,6 +424,24 @@
   </si>
   <si>
     <t xml:space="preserve">NLMO62P72-04 nebo NLA062P72-04  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-32 ~ +40 °C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 DI, 1 AI, 2 PT1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZPĚTNÁ VAZBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x zelená (SERVO OK)  1x červená (SERVO ERROR) 1x zelená (ECAT RUN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 10pin WEIDMÜLLER  BLZP 5.08HC/10/180F </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 5pin WEIDMÜLLER  BCZ 3.81/05/180F  </t>
   </si>
   <si>
     <t xml:space="preserve">0-320 VDC (pojistka 10 A)</t>
@@ -1081,7 +1100,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1100,6 +1119,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2180,7 +2203,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2406,6 +2429,255 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.88"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2443,7 +2715,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,7 +2723,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2467,7 +2739,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,7 +2747,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,7 +2859,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2603,7 +2875,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2633,14 +2905,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -2671,7 +2943,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2679,7 +2951,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2695,7 +2967,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2815,7 +3087,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2831,7 +3103,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2861,7 +3133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2899,7 +3171,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2907,7 +3179,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2915,7 +3187,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2923,7 +3195,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2936,10 +3208,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3059,7 +3331,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3075,7 +3347,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3109,7 +3381,7 @@
         <v>122</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3123,7 +3395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3161,7 +3433,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3169,7 +3441,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3177,7 +3449,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3198,10 +3470,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3321,7 +3593,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3337,7 +3609,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3371,7 +3643,7 @@
         <v>122</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3385,7 +3657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3423,7 +3695,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3431,7 +3703,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3439,7 +3711,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3447,7 +3719,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3460,10 +3732,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3583,7 +3855,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3599,7 +3871,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3633,269 +3905,7 @@
         <v>122</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B32"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -4153,76 +4163,76 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4242,137 +4252,158 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+    </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="B24" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>159</v>
+      <c r="B25" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>160</v>
+      <c r="B26" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>161</v>
+      <c r="B27" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>162</v>
+      <c r="B28" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>163</v>
-      </c>
+      <c r="B29" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>121</v>
       </c>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>164</v>
+      <c r="B32" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -4416,7 +4447,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4424,7 +4455,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4432,7 +4463,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4440,7 +4471,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4448,7 +4479,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4456,7 +4487,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4464,7 +4495,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4517,7 +4548,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -4568,7 +4599,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4576,7 +4607,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4584,7 +4615,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4592,7 +4623,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4600,7 +4631,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4613,7 +4644,7 @@
         <v>122</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -4657,7 +4688,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4665,7 +4696,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4673,7 +4704,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4681,7 +4712,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4689,7 +4720,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4697,7 +4728,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4705,7 +4736,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4758,7 +4789,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -4809,7 +4840,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4817,7 +4848,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4825,7 +4856,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4833,7 +4864,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4841,7 +4872,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4854,7 +4885,7 @@
         <v>122</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -4869,6 +4900,247 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4898,7 +5170,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4906,7 +5178,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4914,7 +5186,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4922,7 +5194,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4930,7 +5202,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4946,7 +5218,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4999,7 +5271,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -5050,7 +5322,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5058,7 +5330,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5074,7 +5346,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5082,7 +5354,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5090,7 +5362,7 @@
         <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5103,7 +5375,7 @@
         <v>122</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -5117,7 +5389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5145,46 +5417,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -5193,43 +5465,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -5253,7 +5525,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -5261,18 +5533,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5288,12 +5560,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -5301,26 +5573,26 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -5334,7 +5606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5362,43 +5634,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>49</v>
@@ -5410,43 +5682,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -5470,7 +5742,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -5478,18 +5750,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5505,12 +5777,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -5521,39 +5793,39 @@
         <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -5567,7 +5839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5598,21 +5870,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>49</v>
@@ -5621,16 +5893,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>49</v>
@@ -5639,7 +5911,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>59</v>
@@ -5651,22 +5923,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -5675,19 +5947,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C12" s="4"/>
     </row>
@@ -5711,7 +5983,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -5719,18 +5991,18 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5746,12 +6018,12 @@
         <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>1</v>
@@ -5762,239 +6034,47 @@
         <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -6036,28 +6116,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -6084,19 +6164,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>239</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>241</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>242</v>
       </c>
       <c r="C9" s="4"/>
     </row>
@@ -6111,84 +6191,82 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>200</v>
+        <v>249</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="C16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>206</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>247</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>251</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>100</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>104</v>
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>105</v>
+      <c r="A21" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -6207,7 +6285,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
@@ -6230,28 +6308,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -6305,10 +6383,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -6326,10 +6404,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C14" s="4"/>
     </row>
@@ -6338,7 +6416,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -6347,18 +6425,42 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>251</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>247</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -6605,6 +6707,176 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -6626,107 +6898,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6734,16 +7006,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>2.05</v>
@@ -6769,16 +7041,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2.05</v>
@@ -6804,16 +7076,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>2.05</v>
@@ -6839,16 +7111,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>2.05</v>
@@ -6874,16 +7146,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>2.05</v>
@@ -6909,16 +7181,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2.05</v>
@@ -6944,16 +7216,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1.25</v>
@@ -6979,16 +7251,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>1.25</v>
@@ -7020,7 +7292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -7045,89 +7317,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7147,7 +7419,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>300</v>
@@ -7176,7 +7448,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>300</v>
@@ -7205,7 +7477,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>300</v>
@@ -7234,7 +7506,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>300</v>
@@ -7263,7 +7535,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>300</v>
@@ -7292,7 +7564,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>300</v>
@@ -7315,7 +7587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -7336,44 +7608,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7381,7 +7653,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>11</v>
@@ -7395,7 +7667,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>11</v>

</xml_diff>

<commit_message>
Deployed 85df940c with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/parameters.xlsx
+++ b/Manual/source/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,25 +22,27 @@
     <sheet name="TGZ-S-48-100_425-O" sheetId="12" state="visible" r:id="rId14"/>
     <sheet name="TGZ-S-230-5_15" sheetId="13" state="visible" r:id="rId15"/>
     <sheet name="TGZ-S-230-5_15-UNI-RI" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="TGZ-D-320-5_10" sheetId="15" state="visible" r:id="rId17"/>
-    <sheet name="TGZ-D-320-5_15" sheetId="16" state="visible" r:id="rId18"/>
-    <sheet name="TGZ-S-400-3_9" sheetId="17" state="visible" r:id="rId19"/>
-    <sheet name="TGZ-S-400-7_15" sheetId="18" state="visible" r:id="rId20"/>
-    <sheet name="TGZ-S-400-10_20" sheetId="19" state="visible" r:id="rId21"/>
-    <sheet name="TGZ-S-400-14_30" sheetId="20" state="visible" r:id="rId22"/>
-    <sheet name="TGZ-D-560-3_9" sheetId="21" state="visible" r:id="rId23"/>
-    <sheet name="TGZ-D-560-7_15" sheetId="22" state="visible" r:id="rId24"/>
-    <sheet name="TGZ-D-560-10_20" sheetId="23" state="visible" r:id="rId25"/>
-    <sheet name="TGZ-D-560-30_50" sheetId="24" state="visible" r:id="rId26"/>
-    <sheet name="TGS-320-10_15" sheetId="25" state="visible" r:id="rId27"/>
-    <sheet name="TGS-560-25_50" sheetId="26" state="visible" r:id="rId28"/>
-    <sheet name="TGS-560-50_100" sheetId="27" state="visible" r:id="rId29"/>
-    <sheet name="TGMmini" sheetId="28" state="visible" r:id="rId30"/>
-    <sheet name="TGMcontroller" sheetId="29" state="visible" r:id="rId31"/>
-    <sheet name="TGZpMotion" sheetId="30" state="visible" r:id="rId32"/>
-    <sheet name="commonHW_DI" sheetId="31" state="visible" r:id="rId33"/>
-    <sheet name="commonHW_DO" sheetId="32" state="visible" r:id="rId34"/>
-    <sheet name="commonHW_AI" sheetId="33" state="visible" r:id="rId35"/>
+    <sheet name="TGZ-S-400-14_30-UNI-RI" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="TGZ-S-400-14_30-RI" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="TGZ-D-320-5_10" sheetId="17" state="visible" r:id="rId19"/>
+    <sheet name="TGZ-D-320-5_15" sheetId="18" state="visible" r:id="rId20"/>
+    <sheet name="TGZ-S-400-3_9" sheetId="19" state="visible" r:id="rId21"/>
+    <sheet name="TGZ-S-400-7_15" sheetId="20" state="visible" r:id="rId22"/>
+    <sheet name="TGZ-S-400-10_20" sheetId="21" state="visible" r:id="rId23"/>
+    <sheet name="TGZ-S-400-14_30" sheetId="22" state="visible" r:id="rId24"/>
+    <sheet name="TGZ-D-560-3_9" sheetId="23" state="visible" r:id="rId25"/>
+    <sheet name="TGZ-D-560-7_15" sheetId="24" state="visible" r:id="rId26"/>
+    <sheet name="TGZ-D-560-10_20" sheetId="25" state="visible" r:id="rId27"/>
+    <sheet name="TGZ-D-560-30_50" sheetId="26" state="visible" r:id="rId28"/>
+    <sheet name="TGS-320-10_15" sheetId="27" state="visible" r:id="rId29"/>
+    <sheet name="TGS-560-25_50" sheetId="28" state="visible" r:id="rId30"/>
+    <sheet name="TGS-560-50_100" sheetId="29" state="visible" r:id="rId31"/>
+    <sheet name="TGMmini" sheetId="30" state="visible" r:id="rId32"/>
+    <sheet name="TGMcontroller" sheetId="31" state="visible" r:id="rId33"/>
+    <sheet name="TGZpMotion" sheetId="32" state="visible" r:id="rId34"/>
+    <sheet name="commonHW_DI" sheetId="33" state="visible" r:id="rId35"/>
+    <sheet name="commonHW_DO" sheetId="34" state="visible" r:id="rId36"/>
+    <sheet name="commonHW_AI" sheetId="35" state="visible" r:id="rId37"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="313">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -444,6 +446,39 @@
     <t xml:space="preserve">1 x 5pin WEIDMÜLLER  BCZ 3.81/05/180F  </t>
   </si>
   <si>
+    <t xml:space="preserve">3 x 400 VAC/50Hz 20A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,9 kVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pracovní spínací frekvence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 kHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 12pin WEIDMÜLLER BLZ 7.62HP/12/180F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 5pin WEIDMÜLLER  BCZ 3.81/05/180F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 6pin WEIDMÜLLER  BLF 7.62HP/06/180F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCZXX3P49-04</t>
+  </si>
+  <si>
     <t xml:space="preserve">0-320 VDC (pojistka 10 A)</t>
   </si>
   <si>
@@ -474,21 +509,9 @@
     <t xml:space="preserve">9 A</t>
   </si>
   <si>
-    <t xml:space="preserve">Pracovní spínací frekvence</t>
-  </si>
-  <si>
     <t xml:space="preserve">20 kHz</t>
   </si>
   <si>
-    <t xml:space="preserve">1 x 12pin WEIDMÜLLER BLZ 7.62HP/12/180F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 x 6pin WEIDMÜLLER  BLF 7.62HP/06/180F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NCZXX3P49-04</t>
-  </si>
-  <si>
     <t xml:space="preserve">3 x 400 VAC/50Hz 10A</t>
   </si>
   <si>
@@ -510,24 +533,6 @@
     <t xml:space="preserve">20 A</t>
   </si>
   <si>
-    <t xml:space="preserve">3 x 400 VAC/50Hz 20A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,9 kVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110 W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 kHz</t>
-  </si>
-  <si>
     <t xml:space="preserve">24 VDC ± 10 %, 2 A*</t>
   </si>
   <si>
@@ -595,9 +600,6 @@
   </si>
   <si>
     <t xml:space="preserve">šroubovací svorky M8x12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 x 5pin WEIDMÜLLER  BCZ 3.81/05/180F</t>
   </si>
   <si>
     <t xml:space="preserve">2 x 4pin  WEIDMÜLLER LSF</t>
@@ -1100,7 +1102,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1119,10 +1121,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2435,14 +2433,14 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2513,7 +2511,7 @@
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2678,6 +2676,510 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.89"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.89"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2715,7 +3217,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2723,7 +3225,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2739,7 +3241,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2747,7 +3249,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,7 +3361,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2875,7 +3377,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,7 +3407,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2943,7 +3445,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2951,7 +3453,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2967,7 +3469,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3087,7 +3589,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3103,7 +3605,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3120,530 +3622,6 @@
       </c>
       <c r="B29" s="1" t="s">
         <v>105</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B32"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B32"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3695,7 +3673,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3703,7 +3681,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3711,7 +3689,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3719,7 +3697,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3727,15 +3705,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3855,7 +3833,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3871,7 +3849,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3905,7 +3883,7 @@
         <v>122</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4163,7 +4141,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4217,7 +4195,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>155</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4225,15 +4203,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>156</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4353,7 +4331,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4369,7 +4347,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4403,7 +4381,7 @@
         <v>122</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4425,77 +4403,77 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>162</v>
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>163</v>
+      <c r="A8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4514,137 +4492,158 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+    </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="B24" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>165</v>
+      <c r="B25" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>166</v>
+      <c r="B26" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>167</v>
+      <c r="B27" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>168</v>
+      <c r="B28" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>169</v>
-      </c>
+      <c r="B29" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>121</v>
       </c>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>170</v>
+      <c r="B32" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4666,77 +4665,77 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="58.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>158</v>
+      <c r="B2" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>159</v>
+      <c r="B3" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>171</v>
+      <c r="B4" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>147</v>
+      <c r="B5" s="4" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>154</v>
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>172</v>
+      <c r="A8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4755,137 +4754,158 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+    </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="B24" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>165</v>
+      <c r="B25" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>166</v>
+      <c r="B26" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>167</v>
+      <c r="B27" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>168</v>
+      <c r="B28" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>169</v>
-      </c>
+      <c r="B29" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>121</v>
       </c>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>170</v>
+      <c r="B32" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4929,7 +4949,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4937,7 +4957,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4945,7 +4965,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4953,7 +4973,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4961,7 +4981,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4969,7 +4989,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4977,7 +4997,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5030,7 +5050,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -5081,7 +5101,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5089,7 +5109,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5097,7 +5117,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5105,7 +5125,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5113,7 +5133,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5126,7 +5146,7 @@
         <v>122</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -5141,6 +5161,488 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5170,7 +5672,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5178,7 +5680,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5186,7 +5688,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5194,7 +5696,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5202,7 +5704,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5218,7 +5720,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5271,7 +5773,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -5322,7 +5824,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5330,7 +5832,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5354,7 +5856,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5362,7 +5864,7 @@
         <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5389,7 +5891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5429,7 +5931,7 @@
         <v>186</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -5465,7 +5967,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="C7" s="4"/>
     </row>
@@ -5576,7 +6078,7 @@
         <v>207</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5606,7 +6108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5709,7 +6211,7 @@
         <v>197</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C10" s="4"/>
     </row>
@@ -5793,7 +6295,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5839,7 +6341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5870,7 +6372,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5950,7 +6452,7 @@
         <v>197</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -6034,7 +6536,7 @@
         <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6050,7 +6552,7 @@
         <v>208</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6075,392 +6577,6 @@
       </c>
       <c r="B29" s="1" t="s">
         <v>233</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -6707,6 +6823,392 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -6872,7 +7374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -7292,7 +7794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -7587,7 +8089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>

</xml_diff>

<commit_message>
Deployed d9f29a86 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/parameters.xlsx
+++ b/Manual/source/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="37"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -45,6 +45,7 @@
     <sheet name="commonHW_DI" sheetId="35" state="visible" r:id="rId37"/>
     <sheet name="commonHW_DO" sheetId="36" state="visible" r:id="rId38"/>
     <sheet name="commonHW_AI" sheetId="37" state="visible" r:id="rId39"/>
+    <sheet name="TGmonitor7" sheetId="38" state="visible" r:id="rId40"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1837" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="332">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -1022,13 +1023,72 @@
   <si>
     <t xml:space="preserve">us</t>
   </si>
+  <si>
+    <t xml:space="preserve">Doporučený nap. zdroj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min. 300 mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPLEJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uhlopříčka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 palců</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pozoravací úhly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170 °</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rozlišení</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1024 x 600 px</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rozměr zobrazovací plochy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">154,21 x 85,92 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rozteč pixelů</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150,6(H) x 143,2(V) um</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barevný gamut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45% NTSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximální jas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 cd/m²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kontrast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800:1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00\ %"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1104,7 +1164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1123,6 +1183,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2920,7 +2988,7 @@
   </sheetPr>
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -8660,6 +8728,185 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">

</xml_diff>

<commit_message>
Deployed 5e95b993 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/parameters.xlsx
+++ b/Manual/source/tab/parameters.xlsx
@@ -12,10 +12,10 @@
     <sheet name="TGZ-D-48-50_100" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="TGZ-S-48-50_100" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="TGZ-S-48-50_100-UNI-RI" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="TGZ-S-48-50_100RI" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="TGZ-S-48-100_250RI" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="TGZ-S-48-50_100-RI" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="TGZ-S-48-100_250-RI" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="TGZ-S-48-100_250-UNI-RI" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="TGZ-S-48-100_300RI" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="TGZ-S-48-100_300-RI" sheetId="8" state="visible" r:id="rId10"/>
     <sheet name="TGZ-S-48-100_300-UNI-RI" sheetId="9" state="visible" r:id="rId11"/>
     <sheet name="TGZ-S-48-100_250" sheetId="10" state="visible" r:id="rId12"/>
     <sheet name="TGZ-S-48-100_250-O" sheetId="11" state="visible" r:id="rId13"/>
@@ -9652,7 +9652,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Deployed e03e28a2 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/parameters.xlsx
+++ b/Manual/source/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -44,10 +44,11 @@
     <sheet name="TGMmini" sheetId="34" state="visible" r:id="rId36"/>
     <sheet name="TGMcontroller" sheetId="35" state="visible" r:id="rId37"/>
     <sheet name="TGZpMotion" sheetId="36" state="visible" r:id="rId38"/>
-    <sheet name="commonHW_DI" sheetId="37" state="visible" r:id="rId39"/>
-    <sheet name="commonHW_DO" sheetId="38" state="visible" r:id="rId40"/>
-    <sheet name="commonHW_AI" sheetId="39" state="visible" r:id="rId41"/>
-    <sheet name="TGmonitor7" sheetId="40" state="visible" r:id="rId42"/>
+    <sheet name="X8_commonHW_DI_tab" sheetId="37" state="visible" r:id="rId39"/>
+    <sheet name="X8_commonHW_DI_RI_tab" sheetId="38" state="visible" r:id="rId40"/>
+    <sheet name="X8_commonHW_DO_tab" sheetId="39" state="visible" r:id="rId41"/>
+    <sheet name="X8_commonHW_AI_tab" sheetId="40" state="visible" r:id="rId42"/>
+    <sheet name="TGmonitor7" sheetId="41" state="visible" r:id="rId43"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="332">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -8820,6 +8821,392 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="26.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="30.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -9097,106 +9484,6 @@
       </c>
       <c r="I9" s="1" t="n">
         <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.24"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -9470,6 +9757,106 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -10394,7 +10781,7 @@
   </sheetPr>
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Deployed 66002b25 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/parameters.xlsx
+++ b/Manual/source/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="39"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -15,11 +15,11 @@
     <sheet name="TGZ-S-48-50_100-RI" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="TGZ-S-48-100_250-RI" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="TGZ-S-48-100_250-UNI-RI" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="TGZ-S-48-100_300-RI" sheetId="8" state="visible" r:id="rId10"/>
-    <sheet name="TGZ-S-48-100_300-UNI-RI" sheetId="9" state="visible" r:id="rId11"/>
-    <sheet name="TGZ-S-48-100_250" sheetId="10" state="visible" r:id="rId12"/>
-    <sheet name="TGZ-S-48-100_250-O" sheetId="11" state="visible" r:id="rId13"/>
-    <sheet name="TGZ-S-48-100_300" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="TGZ-S-48-100_300" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="TGZ-S-48-100_300-RI" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="TGZ-S-48-100_300-UNI-RI" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="TGZ-S-48-100_250" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="TGZ-S-48-100_250-O" sheetId="12" state="visible" r:id="rId14"/>
     <sheet name="TGZ-S-48-100_300-O" sheetId="13" state="visible" r:id="rId15"/>
     <sheet name="TGZ-S-48-100_425" sheetId="14" state="visible" r:id="rId16"/>
     <sheet name="TGZ-S-48-100_425-O" sheetId="15" state="visible" r:id="rId17"/>
@@ -359,19 +359,19 @@
     <t xml:space="preserve">1 x 4pin MOLEX Micro-Fit 3.0, 430250400</t>
   </si>
   <si>
-    <t xml:space="preserve">300 A</t>
+    <t xml:space="preserve">350 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 x Pressfit M5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 5pin MOLEX Micro-Fit 3.0, 436450500</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 22pin WEIDMÜLLER  B2CF 3.50/22/180</t>
   </si>
   <si>
     <t xml:space="preserve">1 x zelená (SERVO OK)  1x červená (SERVO ERROR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 x Pressfit M5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 x 5pin MOLEX Micro-Fit 3.0, 436450500</t>
   </si>
   <si>
     <t xml:space="preserve">2 x 8pin WEIDMÜLLER  B2CF 3.50/08/180</t>
@@ -1547,6 +1547,266 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1676,7 +1936,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1700,7 +1960,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1716,7 +1976,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,7 +1984,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1778,7 +2038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1912,7 +2172,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1936,7 +2196,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,242 +2269,6 @@
       </c>
       <c r="B31" s="1" t="s">
         <v>107</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B30"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2265,8 +2289,8 @@
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J30" activeCellId="0" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2392,7 +2416,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2416,7 +2440,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2676,7 +2700,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2684,7 +2708,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2872,7 +2896,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2896,7 +2920,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8196,7 +8220,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8382,7 +8406,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -9759,7 +9783,7 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -10779,15 +10803,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
   </cols>
   <sheetData>
@@ -10828,7 +10852,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10860,7 +10884,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10873,138 +10897,130 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>1</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>94</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="1" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -11023,10 +11039,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11072,7 +11088,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11117,153 +11133,137 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>74</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>94</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="1" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deployed 01c10f05 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/parameters.xlsx
+++ b/Manual/source/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="334">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -346,7 +346,7 @@
     <t xml:space="preserve">Řízení, STO</t>
   </si>
   <si>
-    <t xml:space="preserve">1 x 5pin MOLEX Micro-Lock, 5055700501</t>
+    <t xml:space="preserve">1 x 5pin Molex Micro-Fit 3.0 - 436450500</t>
   </si>
   <si>
     <t xml:space="preserve">3 x Pressfit M8</t>
@@ -371,9 +371,6 @@
   </si>
   <si>
     <t xml:space="preserve">8 x Pressfit M5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 x 5pin MOLEX Micro-Fit 3.0, 436450500</t>
   </si>
   <si>
     <t xml:space="preserve">1 x 22pin WEIDMÜLLER  B2CF 3.50/22/180</t>
@@ -1561,7 +1558,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1805,7 +1802,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2064,8 +2061,8 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2191,7 +2188,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2215,7 +2212,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2239,7 +2236,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2263,7 +2260,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2271,7 +2268,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2427,7 +2424,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,7 +2448,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2467,7 +2464,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,7 +2472,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2483,7 +2480,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2491,7 +2488,7 @@
         <v>55</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,7 +2496,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2507,7 +2504,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2515,15 +2512,15 @@
         <v>96</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2671,7 +2668,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2695,7 +2692,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2711,7 +2708,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,7 +2716,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2727,7 +2724,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,7 +2732,7 @@
         <v>55</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2743,7 +2740,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2751,7 +2748,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2759,15 +2756,15 @@
         <v>96</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2789,7 +2786,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2843,7 +2840,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2963,7 +2960,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3079,7 +3076,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3151,7 +3148,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3175,7 +3172,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3191,7 +3188,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3199,7 +3196,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3207,7 +3204,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3215,7 +3212,7 @@
         <v>55</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3223,7 +3220,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3231,7 +3228,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3239,15 +3236,15 @@
         <v>96</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3291,7 +3288,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3299,7 +3296,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,7 +3304,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3315,7 +3312,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3331,7 +3328,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3435,7 +3432,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3443,7 +3440,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3451,7 +3448,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3459,7 +3456,7 @@
         <v>42</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3467,21 +3464,21 @@
         <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3525,7 +3522,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3533,7 +3530,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3541,7 +3538,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3549,7 +3546,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3565,7 +3562,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3681,7 +3678,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3689,7 +3686,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3697,7 +3694,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3705,7 +3702,7 @@
         <v>42</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3713,7 +3710,7 @@
         <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3721,16 +3718,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6774,7 +6771,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6782,7 +6779,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6790,7 +6787,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6798,7 +6795,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6814,7 +6811,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6830,7 +6827,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6883,7 +6880,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>74</v>
@@ -6891,7 +6888,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>1</v>
@@ -6934,7 +6931,7 @@
         <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6950,7 +6947,7 @@
         <v>36</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6958,7 +6955,7 @@
         <v>38</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6966,21 +6963,21 @@
         <v>40</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -7260,7 +7257,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7268,7 +7265,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7276,7 +7273,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7284,7 +7281,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7300,7 +7297,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7316,7 +7313,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7353,7 +7350,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>74</v>
@@ -7361,7 +7358,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>1</v>
@@ -7404,7 +7401,7 @@
         <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7420,7 +7417,7 @@
         <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7428,7 +7425,7 @@
         <v>38</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7436,21 +7433,21 @@
         <v>40</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -7502,7 +7499,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7510,7 +7507,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7518,7 +7515,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7526,7 +7523,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7534,15 +7531,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7558,7 +7555,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7614,7 +7611,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>74</v>
@@ -7622,7 +7619,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>1</v>
@@ -7665,7 +7662,7 @@
         <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7681,7 +7678,7 @@
         <v>36</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7689,7 +7686,7 @@
         <v>38</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7697,21 +7694,21 @@
         <v>40</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -7763,7 +7760,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7771,7 +7768,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7779,7 +7776,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7787,7 +7784,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7795,15 +7792,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7819,7 +7816,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7859,7 +7856,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>74</v>
@@ -7867,7 +7864,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>1</v>
@@ -7910,7 +7907,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7926,7 +7923,7 @@
         <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7934,7 +7931,7 @@
         <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7942,21 +7939,21 @@
         <v>40</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -8008,7 +8005,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8016,7 +8013,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8024,7 +8021,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8032,7 +8029,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8040,7 +8037,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8152,7 +8149,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8160,7 +8157,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8168,7 +8165,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8176,7 +8173,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8184,7 +8181,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -8236,7 +8233,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8244,7 +8241,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8252,7 +8249,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8260,7 +8257,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8380,7 +8377,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8388,7 +8385,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8396,7 +8393,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8404,7 +8401,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8412,7 +8409,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -8464,7 +8461,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8472,7 +8469,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8480,7 +8477,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8488,7 +8485,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8501,10 +8498,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8624,7 +8621,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8632,7 +8629,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8640,7 +8637,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8648,7 +8645,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8656,7 +8653,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8665,16 +8662,16 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -8726,7 +8723,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8734,7 +8731,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8742,7 +8739,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8763,10 +8760,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8886,7 +8883,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8894,7 +8891,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8902,7 +8899,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8910,7 +8907,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8918,7 +8915,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8927,16 +8924,16 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -8988,7 +8985,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8996,7 +8993,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9004,7 +9001,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9012,7 +9009,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9025,10 +9022,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9148,7 +9145,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9156,7 +9153,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9164,7 +9161,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9172,7 +9169,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9180,7 +9177,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9189,16 +9186,16 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -9250,7 +9247,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9258,7 +9255,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9266,7 +9263,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9274,7 +9271,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9282,15 +9279,15 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9410,7 +9407,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9418,7 +9415,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9426,7 +9423,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9434,7 +9431,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9442,7 +9439,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9451,16 +9448,16 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -9504,7 +9501,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9512,7 +9509,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9520,7 +9517,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9528,7 +9525,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9536,7 +9533,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9544,7 +9541,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9552,7 +9549,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9605,7 +9602,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -9656,7 +9653,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9664,7 +9661,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9672,7 +9669,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9680,7 +9677,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9688,20 +9685,20 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -9973,7 +9970,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9981,7 +9978,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9989,7 +9986,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9997,7 +9994,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10005,7 +10002,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10021,7 +10018,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10074,7 +10071,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -10125,7 +10122,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10133,7 +10130,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10141,7 +10138,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10149,7 +10146,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10157,20 +10154,20 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -10214,7 +10211,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10222,7 +10219,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10230,7 +10227,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10238,7 +10235,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10246,7 +10243,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10254,7 +10251,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10262,7 +10259,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10315,7 +10312,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -10366,7 +10363,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10374,7 +10371,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10382,7 +10379,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10390,7 +10387,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10398,20 +10395,20 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -10455,7 +10452,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10463,7 +10460,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10471,7 +10468,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10479,7 +10476,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10487,7 +10484,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10503,7 +10500,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10556,7 +10553,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -10607,7 +10604,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10615,7 +10612,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10631,7 +10628,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10639,7 +10636,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10647,20 +10644,20 @@
         <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -10702,46 +10699,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -10750,43 +10747,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -10810,7 +10807,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
@@ -10818,18 +10815,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10845,12 +10842,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>1</v>
@@ -10858,26 +10855,26 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -10919,43 +10916,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -10967,43 +10964,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -11027,7 +11024,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
@@ -11035,18 +11032,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11062,12 +11059,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>1</v>
@@ -11078,39 +11075,39 @@
         <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -11155,21 +11152,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>49</v>
@@ -11178,16 +11175,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -11196,7 +11193,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>59</v>
@@ -11208,22 +11205,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -11232,19 +11229,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -11268,7 +11265,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -11276,18 +11273,18 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11303,12 +11300,12 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>1</v>
@@ -11319,47 +11316,47 @@
         <v>38</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -11401,28 +11398,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -11449,19 +11446,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -11476,28 +11473,28 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -11515,16 +11512,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>253</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>1</v>
@@ -11532,10 +11529,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11543,15 +11540,15 @@
         <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -11593,28 +11590,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -11668,10 +11665,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -11689,10 +11686,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -11701,7 +11698,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -11710,7 +11707,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>39</v>
@@ -11721,7 +11718,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11729,7 +11726,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11737,7 +11734,7 @@
         <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11745,7 +11742,7 @@
         <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -11787,28 +11784,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -11862,10 +11859,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -11883,10 +11880,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -11895,7 +11892,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -11907,7 +11904,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11915,7 +11912,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -11955,107 +11952,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12063,16 +12060,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2.05</v>
@@ -12098,16 +12095,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>2.05</v>
@@ -12133,16 +12130,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>2.05</v>
@@ -12168,16 +12165,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>2.05</v>
@@ -12203,16 +12200,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>2.05</v>
@@ -12238,16 +12235,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2.05</v>
@@ -12273,16 +12270,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>1.25</v>
@@ -12308,16 +12305,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>1.25</v>
@@ -12629,98 +12626,98 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12728,10 +12725,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>24</v>
@@ -12760,10 +12757,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>24</v>
@@ -12792,10 +12789,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>24</v>
@@ -12824,10 +12821,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>24</v>
@@ -12856,10 +12853,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>24</v>
@@ -12888,10 +12885,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>24</v>
@@ -12920,10 +12917,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>24</v>
@@ -12952,10 +12949,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>24</v>
@@ -13015,89 +13012,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="H3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13117,7 +13114,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>300</v>
@@ -13146,7 +13143,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>300</v>
@@ -13175,7 +13172,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>300</v>
@@ -13204,7 +13201,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>300</v>
@@ -13233,7 +13230,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>300</v>
@@ -13262,7 +13259,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>300</v>
@@ -13306,44 +13303,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13351,7 +13348,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>11</v>
@@ -13365,7 +13362,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>11</v>
@@ -13413,24 +13410,24 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -13438,32 +13435,32 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -13471,66 +13468,66 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>323</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>329</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>333</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13811,7 +13808,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14055,7 +14052,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14314,8 +14311,8 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14583,7 +14580,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14757,7 +14754,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Deployed 8bee31b9 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/parameters.xlsx
+++ b/Manual/source/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,28 +29,29 @@
     <sheet name="TGZ-S-230-5_15-UNI-RI" sheetId="19" state="visible" r:id="rId21"/>
     <sheet name="TGZ-S-230-5_15-RI" sheetId="20" state="visible" r:id="rId22"/>
     <sheet name="TGZ-S-400-14_30-UNI-RI" sheetId="21" state="visible" r:id="rId23"/>
-    <sheet name="TGZ-S-400-14_30-RI" sheetId="22" state="visible" r:id="rId24"/>
-    <sheet name="TGZ-D-320-5_10" sheetId="23" state="visible" r:id="rId25"/>
-    <sheet name="TGZ-D-320-5_15" sheetId="24" state="visible" r:id="rId26"/>
-    <sheet name="TGZ-S-400-3_9" sheetId="25" state="visible" r:id="rId27"/>
-    <sheet name="TGZ-S-400-7_15" sheetId="26" state="visible" r:id="rId28"/>
-    <sheet name="TGZ-S-400-10_20" sheetId="27" state="visible" r:id="rId29"/>
-    <sheet name="TGZ-S-400-14_30" sheetId="28" state="visible" r:id="rId30"/>
-    <sheet name="TGZ-D-560-3_9" sheetId="29" state="visible" r:id="rId31"/>
-    <sheet name="TGZ-D-560-7_15" sheetId="30" state="visible" r:id="rId32"/>
-    <sheet name="TGZ-D-560-10_20" sheetId="31" state="visible" r:id="rId33"/>
-    <sheet name="TGZ-D-560-30_50" sheetId="32" state="visible" r:id="rId34"/>
-    <sheet name="TGS-320-10_15" sheetId="33" state="visible" r:id="rId35"/>
-    <sheet name="TGS-560-25_50" sheetId="34" state="visible" r:id="rId36"/>
-    <sheet name="TGS-560-50_100" sheetId="35" state="visible" r:id="rId37"/>
-    <sheet name="TGMmini" sheetId="36" state="visible" r:id="rId38"/>
-    <sheet name="TGMcontroller" sheetId="37" state="visible" r:id="rId39"/>
-    <sheet name="TGZpMotion" sheetId="38" state="visible" r:id="rId40"/>
-    <sheet name="X8_commonHW_DI_tab" sheetId="39" state="visible" r:id="rId41"/>
-    <sheet name="X8_commonHW_DI_RI_tab" sheetId="40" state="visible" r:id="rId42"/>
-    <sheet name="X8_commonHW_DO_tab" sheetId="41" state="visible" r:id="rId43"/>
-    <sheet name="X8_commonHW_AI_tab" sheetId="42" state="visible" r:id="rId44"/>
-    <sheet name="TGmonitor7" sheetId="43" state="visible" r:id="rId45"/>
+    <sheet name="TGZ-S-560-14_30-UNIR-RI" sheetId="22" state="visible" r:id="rId24"/>
+    <sheet name="TGZ-S-400-14_30-RI" sheetId="23" state="visible" r:id="rId25"/>
+    <sheet name="TGZ-D-320-5_10" sheetId="24" state="visible" r:id="rId26"/>
+    <sheet name="TGZ-D-320-5_15" sheetId="25" state="visible" r:id="rId27"/>
+    <sheet name="TGZ-S-400-3_9" sheetId="26" state="visible" r:id="rId28"/>
+    <sheet name="TGZ-S-400-7_15" sheetId="27" state="visible" r:id="rId29"/>
+    <sheet name="TGZ-S-400-10_20" sheetId="28" state="visible" r:id="rId30"/>
+    <sheet name="TGZ-S-400-14_30" sheetId="29" state="visible" r:id="rId31"/>
+    <sheet name="TGZ-D-560-3_9" sheetId="30" state="visible" r:id="rId32"/>
+    <sheet name="TGZ-D-560-7_15" sheetId="31" state="visible" r:id="rId33"/>
+    <sheet name="TGZ-D-560-10_20" sheetId="32" state="visible" r:id="rId34"/>
+    <sheet name="TGZ-D-560-30_50" sheetId="33" state="visible" r:id="rId35"/>
+    <sheet name="TGS-320-10_15" sheetId="34" state="visible" r:id="rId36"/>
+    <sheet name="TGS-560-25_50" sheetId="35" state="visible" r:id="rId37"/>
+    <sheet name="TGS-560-50_100" sheetId="36" state="visible" r:id="rId38"/>
+    <sheet name="TGMmini" sheetId="37" state="visible" r:id="rId39"/>
+    <sheet name="TGMcontroller" sheetId="38" state="visible" r:id="rId40"/>
+    <sheet name="TGZpMotion" sheetId="39" state="visible" r:id="rId41"/>
+    <sheet name="X8_commonHW_DI_tab" sheetId="40" state="visible" r:id="rId42"/>
+    <sheet name="X8_commonHW_DI_RI_tab" sheetId="41" state="visible" r:id="rId43"/>
+    <sheet name="X8_commonHW_DO_tab" sheetId="42" state="visible" r:id="rId44"/>
+    <sheet name="X8_commonHW_AI_tab" sheetId="43" state="visible" r:id="rId45"/>
+    <sheet name="TGmonitor7" sheetId="44" state="visible" r:id="rId46"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="337">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -496,6 +497,18 @@
     <t xml:space="preserve">NCZXX3P49-04</t>
   </si>
   <si>
+    <t xml:space="preserve">0 ~ 560 VDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,9 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB1, FB2, FB3, FB4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 x 10pin MOLEX 5031481090 CLIK-MATE 1.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">0-320 VDC (pojistka 10 A)</t>
   </si>
   <si>
@@ -548,9 +561,6 @@
   </si>
   <si>
     <t xml:space="preserve">24 VDC ± 10 %, 2 A*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 ~ 560 VDC</t>
   </si>
   <si>
     <t xml:space="preserve">3,4 kVA</t>
@@ -2061,7 +2071,7 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -7727,6 +7737,267 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.89"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -7967,7 +8238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -8005,7 +8276,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8013,7 +8284,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8029,7 +8300,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8037,7 +8308,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8149,7 +8420,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8165,7 +8436,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8195,7 +8466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -8233,7 +8504,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8241,7 +8512,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8257,7 +8528,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8377,7 +8648,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8393,7 +8664,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8423,7 +8694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -8461,7 +8732,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8469,7 +8740,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8477,7 +8748,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8485,7 +8756,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8501,7 +8772,7 @@
         <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8685,7 +8956,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -8723,7 +8994,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8731,7 +9002,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8763,7 +9034,7 @@
         <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8947,7 +9218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -8985,7 +9256,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8993,7 +9264,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9001,7 +9272,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9009,7 +9280,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9025,7 +9296,7 @@
         <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9209,7 +9480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -9458,247 +9729,6 @@
       </c>
       <c r="B32" s="4" t="s">
         <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B32"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="45.61"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -9970,7 +10000,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9978,7 +10008,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9986,7 +10016,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9994,7 +10024,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10002,7 +10032,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10010,7 +10040,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10018,7 +10048,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10071,7 +10101,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -10122,7 +10152,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10130,7 +10160,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10138,7 +10168,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10146,7 +10176,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10154,7 +10184,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10167,7 +10197,7 @@
         <v>123</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -10211,7 +10241,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10219,7 +10249,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10227,7 +10257,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10235,7 +10265,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10243,7 +10273,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>177</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10251,7 +10281,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>178</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10259,7 +10289,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10312,7 +10342,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -10363,7 +10393,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10371,7 +10401,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10379,7 +10409,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10387,7 +10417,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10395,7 +10425,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10408,7 +10438,7 @@
         <v>123</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -10423,6 +10453,247 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="45.61"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -10452,7 +10723,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10460,7 +10731,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10468,7 +10739,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10484,7 +10755,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10500,7 +10771,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10553,7 +10824,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -10604,7 +10875,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10628,7 +10899,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10636,7 +10907,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10644,7 +10915,7 @@
         <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10657,7 +10928,7 @@
         <v>123</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -10671,7 +10942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -10699,46 +10970,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -10747,43 +11018,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -10807,7 +11078,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
@@ -10815,18 +11086,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10842,12 +11113,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>1</v>
@@ -10855,26 +11126,26 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -10888,7 +11159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -10916,43 +11187,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -10964,43 +11235,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -11024,7 +11295,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
@@ -11032,18 +11303,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11059,12 +11330,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>1</v>
@@ -11075,39 +11346,39 @@
         <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -11121,7 +11392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -11152,21 +11423,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>49</v>
@@ -11175,16 +11446,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -11193,7 +11464,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>59</v>
@@ -11205,22 +11476,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -11229,19 +11500,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -11265,7 +11536,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -11273,18 +11544,18 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11300,12 +11571,12 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>1</v>
@@ -11321,234 +11592,42 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="45.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="2" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -11590,28 +11669,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -11638,19 +11717,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>244</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>245</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>246</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>247</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -11665,84 +11744,82 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>251</v>
+      </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1</v>
+        <v>255</v>
       </c>
       <c r="C16" s="2"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>211</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>255</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>28</v>
+        <v>256</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>103</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>105</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>106</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -11757,6 +11834,200 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="2" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -11784,28 +12055,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -11859,10 +12130,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -11880,10 +12151,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -11892,7 +12163,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -11904,7 +12175,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11913,426 +12184,6 @@
       </c>
       <c r="B18" s="2" t="s">
         <v>103</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="10.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="20.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="22.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="26.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="31.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="30.24"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K5" s="2" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I9" s="2" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J9" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="J10" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -12606,6 +12457,426 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="22.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="26.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="31.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="30.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -12626,98 +12897,98 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12725,10 +12996,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>24</v>
@@ -12757,10 +13028,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>24</v>
@@ -12789,10 +13060,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>24</v>
@@ -12821,10 +13092,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>24</v>
@@ -12853,10 +13124,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>24</v>
@@ -12885,10 +13156,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>24</v>
@@ -12917,10 +13188,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>24</v>
@@ -12949,10 +13220,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>24</v>
@@ -12987,7 +13258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -13012,89 +13283,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13114,7 +13385,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>300</v>
@@ -13143,7 +13414,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>300</v>
@@ -13172,7 +13443,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>300</v>
@@ -13201,7 +13472,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>300</v>
@@ -13230,7 +13501,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>300</v>
@@ -13259,7 +13530,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>300</v>
@@ -13282,7 +13553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -13303,44 +13574,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13348,7 +13619,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>11</v>
@@ -13362,7 +13633,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>11</v>
@@ -13382,7 +13653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -13410,24 +13681,24 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -13435,32 +13706,32 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -13468,66 +13739,66 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Deployed db22c086 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/Manual/source/tab/parameters.xlsx
+++ b/Manual/source/tab/parameters.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="338">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -507,6 +507,9 @@
   </si>
   <si>
     <t xml:space="preserve">4 x 10pin MOLEX 5031481090 CLIK-MATE 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC16XXX</t>
   </si>
   <si>
     <t xml:space="preserve">0-320 VDC (pojistka 10 A)</t>
@@ -7740,7 +7743,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7979,7 +7982,7 @@
         <v>123</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -8276,7 +8279,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8284,7 +8287,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8300,7 +8303,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8308,7 +8311,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8420,7 +8423,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8436,7 +8439,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8504,7 +8507,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8512,7 +8515,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8528,7 +8531,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8648,7 +8651,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8664,7 +8667,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8732,7 +8735,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8740,7 +8743,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8748,7 +8751,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8756,7 +8759,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8772,7 +8775,7 @@
         <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8994,7 +8997,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9002,7 +9005,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9034,7 +9037,7 @@
         <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9256,7 +9259,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9264,7 +9267,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9272,7 +9275,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9280,7 +9283,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9296,7 +9299,7 @@
         <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10000,7 +10003,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10016,7 +10019,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10024,7 +10027,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10032,7 +10035,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10040,7 +10043,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10048,7 +10051,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10101,7 +10104,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -10152,7 +10155,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10160,7 +10163,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10168,7 +10171,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10176,7 +10179,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10184,7 +10187,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10197,7 +10200,7 @@
         <v>123</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -10241,7 +10244,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10257,7 +10260,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10289,7 +10292,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10342,7 +10345,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -10393,7 +10396,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10401,7 +10404,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10409,7 +10412,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10417,7 +10420,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10425,7 +10428,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10438,7 +10441,7 @@
         <v>123</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -10482,7 +10485,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10498,7 +10501,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10506,7 +10509,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10514,7 +10517,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10522,7 +10525,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10530,7 +10533,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10583,7 +10586,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -10634,7 +10637,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10642,7 +10645,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10650,7 +10653,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10658,7 +10661,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10666,7 +10669,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10679,7 +10682,7 @@
         <v>123</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -10723,7 +10726,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10739,7 +10742,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10755,7 +10758,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10771,7 +10774,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10824,7 +10827,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1</v>
@@ -10875,7 +10878,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10899,7 +10902,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10907,7 +10910,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10915,7 +10918,7 @@
         <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10928,7 +10931,7 @@
         <v>123</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -10970,46 +10973,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -11018,43 +11021,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -11078,7 +11081,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
@@ -11086,18 +11089,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11113,12 +11116,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>1</v>
@@ -11126,26 +11129,26 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -11187,43 +11190,43 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -11235,43 +11238,43 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -11295,7 +11298,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
@@ -11303,18 +11306,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11330,12 +11333,12 @@
         <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>1</v>
@@ -11346,39 +11349,39 @@
         <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -11423,21 +11426,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>49</v>
@@ -11446,16 +11449,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -11464,7 +11467,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>59</v>
@@ -11476,22 +11479,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -11500,19 +11503,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -11536,7 +11539,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -11544,18 +11547,18 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11571,12 +11574,12 @@
         <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>1</v>
@@ -11592,42 +11595,42 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -11669,28 +11672,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -11717,19 +11720,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -11744,28 +11747,28 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -11783,16 +11786,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>1</v>
@@ -11800,10 +11803,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11811,15 +11814,15 @@
         <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -11861,28 +11864,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -11936,10 +11939,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -11957,10 +11960,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -11969,7 +11972,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -11978,7 +11981,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>39</v>
@@ -11989,7 +11992,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12055,28 +12058,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -12130,10 +12133,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -12151,10 +12154,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -12163,7 +12166,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
@@ -12175,7 +12178,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12478,107 +12481,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12586,16 +12589,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2.05</v>
@@ -12621,16 +12624,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>2.05</v>
@@ -12656,16 +12659,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>2.05</v>
@@ -12691,16 +12694,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>2.05</v>
@@ -12726,16 +12729,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>2.05</v>
@@ -12761,16 +12764,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>2.05</v>
@@ -12796,16 +12799,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>1.25</v>
@@ -12831,16 +12834,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>1.25</v>
@@ -12897,98 +12900,98 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12996,10 +12999,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>24</v>
@@ -13028,10 +13031,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>24</v>
@@ -13060,10 +13063,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>24</v>
@@ -13092,10 +13095,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>24</v>
@@ -13124,10 +13127,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>24</v>
@@ -13156,10 +13159,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>24</v>
@@ -13188,10 +13191,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>24</v>
@@ -13220,10 +13223,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>24</v>
@@ -13283,89 +13286,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13385,7 +13388,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>300</v>
@@ -13414,7 +13417,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>300</v>
@@ -13443,7 +13446,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>300</v>
@@ -13472,7 +13475,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>300</v>
@@ -13501,7 +13504,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>300</v>
@@ -13530,7 +13533,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>300</v>
@@ -13574,44 +13577,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13619,7 +13622,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>11</v>
@@ -13633,7 +13636,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>11</v>
@@ -13681,24 +13684,24 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -13706,32 +13709,32 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -13739,66 +13742,66 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>